<commit_message>
Data provider and testng.xml file modification
</commit_message>
<xml_diff>
--- a/src/test/java/DataSources/formData.xlsx
+++ b/src/test/java/DataSources/formData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mkhuseli MPU\Desktop\mandla\s.tyindyi_frmwrk\dataDrivenAutomationFramework\src\test\java\dataSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mkhuseli MPU\Desktop\mandla\s.tyindyi_frmwrk\dataDrivenAutomationFramework\src\test\java\DataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00524714-3BD8-48B6-A318-B4F40D587750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02D7E1E-60E9-433D-A302-29EF6749EBD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2CEE0B70-5C30-4C73-93FD-1CBD652B3820}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{2CEE0B70-5C30-4C73-93FD-1CBD652B3820}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="formTestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>0748146380</t>
   </si>
 </sst>
 </file>
@@ -96,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +424,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,8 +456,11 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>748146380</v>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -460,5 +470,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Seperated the excel reader code
</commit_message>
<xml_diff>
--- a/src/test/java/DataSources/formData.xlsx
+++ b/src/test/java/DataSources/formData.xlsx
@@ -1,51 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mkhuseli MPU\Desktop\mandla\s.tyindyi_frmwrk\dataDrivenAutomationFramework\src\test\java\DataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02D7E1E-60E9-433D-A302-29EF6749EBD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{2CEE0B70-5C30-4C73-93FD-1CBD652B3820}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="formTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Test Case Name</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
     <t>Surname</t>
   </si>
   <si>
+    <t>Test Case Happy Path</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>MobileNumber</t>
+    <t>0748146380</t>
   </si>
   <si>
     <t>Siphamandla</t>
@@ -54,20 +53,14 @@
     <t>Tyindyi</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Male</t>
-  </si>
-  <si>
-    <t>0748146380</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +68,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -99,15 +130,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -140,7 +183,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -152,7 +195,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -199,23 +242,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -251,23 +277,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,23 +428,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60813524-7A9A-435C-976F-ECC4120280C1}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="12.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="28" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="2"/>
+    <col min="17" max="17" width="21.28515625" style="2" customWidth="1"/>
+    <col min="18" max="21" width="37.140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="29.140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="26.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="20.140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="16.140625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="19.140625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="15" style="2" customWidth="1"/>
+    <col min="31" max="31" width="16.85546875" style="2" customWidth="1"/>
+    <col min="32" max="32" width="20.42578125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="18" style="2" customWidth="1"/>
+    <col min="34" max="34" width="48" style="2" customWidth="1"/>
+    <col min="35" max="35" width="15.85546875" style="2" customWidth="1"/>
+    <col min="36" max="37" width="21.42578125" style="2" customWidth="1"/>
+    <col min="38" max="38" width="16.85546875" style="2" customWidth="1"/>
+    <col min="39" max="39" width="18.140625" style="2" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" style="2" customWidth="1"/>
+    <col min="41" max="41" width="17.28515625" style="2" customWidth="1"/>
+    <col min="42" max="42" width="13" style="2" customWidth="1"/>
+    <col min="43" max="43" width="14.42578125" style="2" customWidth="1"/>
+    <col min="44" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,33 +485,35 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:34" s="5" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="AH2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
document for issue tracing
</commit_message>
<xml_diff>
--- a/src/test/java/DataSources/formData.xlsx
+++ b/src/test/java/DataSources/formData.xlsx
@@ -38,9 +38,6 @@
     <t>Surname</t>
   </si>
   <si>
-    <t>Test Case Happy Path</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Test Case 1</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -488,7 +488,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>2</v>
@@ -496,19 +496,19 @@
     </row>
     <row r="2" spans="1:34" s="5" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AH2" s="6"/>
     </row>

</xml_diff>